<commit_message>
complete icdc regression suite
</commit_message>
<xml_diff>
--- a/InputFiles/TC29_Canine_StudyUBC02-AllBreeds_StageOfDisease.xlsx
+++ b/InputFiles/TC29_Canine_StudyUBC02-AllBreeds_StageOfDisease.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945B78ED-9EBB-43FB-AD7D-5E65914041BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C88FD2-5A39-463A-82FA-4AA7B259C3ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -503,7 +503,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>